<commit_message>
Updated the seasonals for the month of July 2024
</commit_message>
<xml_diff>
--- a/Trading_Seasonal.xlsx
+++ b/Trading_Seasonal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python Projects\PyCharmProjects\streamlit-seasonal-insights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6781C835-20E0-4380-AE00-0ED87B4DF62D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E1D4DF-310C-45BD-A833-3B7EADD0DF0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1275" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XAUUSD" sheetId="1" r:id="rId1"/>
@@ -838,7 +838,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1896,7 +1896,7 @@
         <v>-1</v>
       </c>
       <c r="H26" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="8">
         <v>0</v>
@@ -1995,7 +1995,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2925,7 +2925,9 @@
       <c r="G23" s="1">
         <v>-1</v>
       </c>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -3013,8 +3015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF96458-0D0F-4E9E-A898-AD571A0B8FE9}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3945,7 +3947,9 @@
       <c r="G23" s="1">
         <v>-1</v>
       </c>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -4034,7 +4038,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M23"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4970,7 +4974,9 @@
       <c r="G23" s="1">
         <v>1</v>
       </c>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -5059,7 +5065,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M23"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5995,7 +6001,9 @@
       <c r="G23" s="1">
         <v>-1</v>
       </c>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -6032,7 +6040,7 @@
       </c>
       <c r="H24" s="5">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="5">
         <f t="shared" si="0"/>
@@ -6053,6 +6061,1033 @@
       <c r="M24" s="5">
         <f t="shared" si="0"/>
         <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G28" s="9"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="N18 N11 B2:M23">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+      <formula>"Bullish"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+      <formula>"Bearish"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:M24">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>"Bearish"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>"Bullish"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3209A12F-F341-4BD4-A48E-083A1865497A}">
+  <dimension ref="A1:N28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>2003</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2004</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>2005</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>2006</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>2007</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>2008</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>2009</v>
+      </c>
+      <c r="B8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>2010</v>
+      </c>
+      <c r="B9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>2011</v>
+      </c>
+      <c r="B10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M10" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>2012</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>2013</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>2014</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M13" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>2015</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1</v>
+      </c>
+      <c r="M14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>2016</v>
+      </c>
+      <c r="B15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M15" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>2017</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+      <c r="M17" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="L18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1</v>
+      </c>
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L19" s="1">
+        <v>1</v>
+      </c>
+      <c r="M19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1</v>
+      </c>
+      <c r="L20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1</v>
+      </c>
+      <c r="M21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1</v>
+      </c>
+      <c r="M22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3">
+        <v>2024</v>
+      </c>
+      <c r="B23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="5">
+        <f>IF(SUM(B2:B23) &gt;= 1, 1, IF(SUM(B2:B23) &lt;= -1, -1, SUM(B2:B23)))</f>
+        <v>-1</v>
+      </c>
+      <c r="C24" s="5">
+        <f t="shared" ref="C24:M24" si="0">IF(SUM(C2:C23) &gt;= 1, 1, IF(SUM(C2:C23) &lt;= -1, -1, SUM(C2:C23)))</f>
+        <v>1</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F24" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G24" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H24" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I24" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="J24" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L24" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="M24" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -6079,1037 +7114,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3209A12F-F341-4BD4-A48E-083A1865497A}">
-  <dimension ref="A1:N28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="10" max="10" width="10.5546875" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" customWidth="1"/>
-    <col min="13" max="13" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>2003</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I2" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J2" s="1">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1">
-        <v>1</v>
-      </c>
-      <c r="L2" s="1">
-        <v>1</v>
-      </c>
-      <c r="M2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>2004</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>-1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>2005</v>
-      </c>
-      <c r="B4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J4" s="1">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="L4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M4" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>2006</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G5" s="1">
-        <v>-1</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J5" s="1">
-        <v>-1</v>
-      </c>
-      <c r="K5" s="1">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1">
-        <v>1</v>
-      </c>
-      <c r="M5" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>2007</v>
-      </c>
-      <c r="B6" s="1">
-        <v>-1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J6" s="1">
-        <v>1</v>
-      </c>
-      <c r="K6" s="1">
-        <v>1</v>
-      </c>
-      <c r="L6" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M6" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>2008</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I7" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J7" s="1">
-        <v>-1</v>
-      </c>
-      <c r="K7" s="1">
-        <v>-1</v>
-      </c>
-      <c r="L7" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>2009</v>
-      </c>
-      <c r="B8" s="1">
-        <v>-1</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1">
-        <v>1</v>
-      </c>
-      <c r="K8" s="1">
-        <v>1</v>
-      </c>
-      <c r="L8" s="1">
-        <v>1</v>
-      </c>
-      <c r="M8" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>2010</v>
-      </c>
-      <c r="B9" s="1">
-        <v>-1</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G9" s="1">
-        <v>-1</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J9" s="1">
-        <v>1</v>
-      </c>
-      <c r="K9" s="1">
-        <v>1</v>
-      </c>
-      <c r="L9" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>2011</v>
-      </c>
-      <c r="B10" s="1">
-        <v>-1</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J10" s="1">
-        <v>-1</v>
-      </c>
-      <c r="K10" s="1">
-        <v>1</v>
-      </c>
-      <c r="L10" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M10" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>2012</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E11" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F11" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J11" s="1">
-        <v>1</v>
-      </c>
-      <c r="K11" s="1">
-        <v>1</v>
-      </c>
-      <c r="L11" s="1">
-        <v>1</v>
-      </c>
-      <c r="M11" s="1">
-        <v>-1</v>
-      </c>
-      <c r="N11" s="6"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>2013</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1">
-        <v>-1</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F12" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G12" s="1">
-        <v>-1</v>
-      </c>
-      <c r="H12" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I12" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J12" s="1">
-        <v>1</v>
-      </c>
-      <c r="K12" s="1">
-        <v>1</v>
-      </c>
-      <c r="L12" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M12" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>2014</v>
-      </c>
-      <c r="B13" s="1">
-        <v>-1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I13" s="1">
-        <v>1</v>
-      </c>
-      <c r="J13" s="1">
-        <v>-1</v>
-      </c>
-      <c r="K13" s="1">
-        <v>1</v>
-      </c>
-      <c r="L13" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M13" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>2015</v>
-      </c>
-      <c r="B14" s="1">
-        <v>-1</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I14" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J14" s="1">
-        <v>-1</v>
-      </c>
-      <c r="K14" s="1">
-        <v>1</v>
-      </c>
-      <c r="L14" s="1">
-        <v>1</v>
-      </c>
-      <c r="M14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>2016</v>
-      </c>
-      <c r="B15" s="1">
-        <v>-1</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F15" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1">
-        <v>1</v>
-      </c>
-      <c r="I15" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J15" s="1">
-        <v>1</v>
-      </c>
-      <c r="K15" s="1">
-        <v>-1</v>
-      </c>
-      <c r="L15" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M15" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>2017</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E16" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F16" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1">
-        <v>1</v>
-      </c>
-      <c r="I16" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J16" s="1">
-        <v>-1</v>
-      </c>
-      <c r="K16" s="1">
-        <v>-1</v>
-      </c>
-      <c r="L16" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <v>2018</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1">
-        <v>-1</v>
-      </c>
-      <c r="D17" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E17" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1">
-        <v>-1</v>
-      </c>
-      <c r="H17" s="1">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J17" s="1">
-        <v>1</v>
-      </c>
-      <c r="K17" s="1">
-        <v>-1</v>
-      </c>
-      <c r="L17" s="1">
-        <v>1</v>
-      </c>
-      <c r="M17" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <v>2019</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1">
-        <v>-1</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F18" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I18" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J18" s="1">
-        <v>1</v>
-      </c>
-      <c r="K18" s="1">
-        <v>1</v>
-      </c>
-      <c r="L18" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M18" s="1">
-        <v>1</v>
-      </c>
-      <c r="N18" s="6"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
-        <v>2020</v>
-      </c>
-      <c r="B19" s="1">
-        <v>-1</v>
-      </c>
-      <c r="C19" s="1">
-        <v>-1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1">
-        <v>1</v>
-      </c>
-      <c r="H19" s="1">
-        <v>1</v>
-      </c>
-      <c r="I19" s="1">
-        <v>1</v>
-      </c>
-      <c r="J19" s="1">
-        <v>-1</v>
-      </c>
-      <c r="K19" s="1">
-        <v>-1</v>
-      </c>
-      <c r="L19" s="1">
-        <v>1</v>
-      </c>
-      <c r="M19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B20" s="1">
-        <v>-1</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1</v>
-      </c>
-      <c r="F20" s="1">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1">
-        <v>-1</v>
-      </c>
-      <c r="H20" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I20" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J20" s="1">
-        <v>-1</v>
-      </c>
-      <c r="K20" s="1">
-        <v>1</v>
-      </c>
-      <c r="L20" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
-        <v>2022</v>
-      </c>
-      <c r="B21" s="1">
-        <v>-1</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F21" s="1">
-        <v>1</v>
-      </c>
-      <c r="G21" s="1">
-        <v>-1</v>
-      </c>
-      <c r="H21" s="1">
-        <v>1</v>
-      </c>
-      <c r="I21" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J21" s="1">
-        <v>-1</v>
-      </c>
-      <c r="K21" s="1">
-        <v>-1</v>
-      </c>
-      <c r="L21" s="1">
-        <v>1</v>
-      </c>
-      <c r="M21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
-        <v>2023</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1">
-        <v>-1</v>
-      </c>
-      <c r="D22" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E22" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F22" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G22" s="1">
-        <v>1</v>
-      </c>
-      <c r="H22" s="1">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J22" s="1">
-        <v>-1</v>
-      </c>
-      <c r="K22" s="1">
-        <v>-1</v>
-      </c>
-      <c r="L22" s="1">
-        <v>1</v>
-      </c>
-      <c r="M22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3">
-        <v>2024</v>
-      </c>
-      <c r="B23" s="1">
-        <v>-1</v>
-      </c>
-      <c r="C23" s="1">
-        <v>-1</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F23" s="1">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1">
-        <v>1</v>
-      </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="5">
-        <f>IF(SUM(B2:B23) &gt;= 1, 1, IF(SUM(B2:B23) &lt;= -1, -1, SUM(B2:B23)))</f>
-        <v>-1</v>
-      </c>
-      <c r="C24" s="5">
-        <f t="shared" ref="C24:M24" si="0">IF(SUM(C2:C23) &gt;= 1, 1, IF(SUM(C2:C23) &lt;= -1, -1, SUM(C2:C23)))</f>
-        <v>1</v>
-      </c>
-      <c r="D24" s="5">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="E24" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F24" s="5">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="G24" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H24" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I24" s="5">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="J24" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K24" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L24" s="5">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="M24" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G28" s="9"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="N18 N11 B2:M23">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
-      <formula>"Bullish"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
-      <formula>"Bearish"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24:M24">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
-      <formula>"Bearish"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
-      <formula>"Bullish"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0515330-FEE6-49E1-9E50-D1F547E84C77}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8085,7 +8095,9 @@
       <c r="G23" s="1">
         <v>1</v>
       </c>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1">
+        <v>-1</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>

</xml_diff>